<commit_message>
adding format to graphs
</commit_message>
<xml_diff>
--- a/TodoLyPerfTest/load todo.ly report.xlsx
+++ b/TodoLyPerfTest/load todo.ly report.xlsx
@@ -45,9 +45,6 @@
     <t>Counter</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>Create project</t>
-  </si>
-  <si>
-    <t>load dashboard</t>
   </si>
   <si>
     <t>Change Password</t>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>Set work priority</t>
+  </si>
+  <si>
+    <t>Load main page</t>
+  </si>
+  <si>
+    <t>Load dashboard</t>
   </si>
 </sst>
 </file>
@@ -107,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,17 +115,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,6 +171,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Load main page</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -205,11 +241,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="137468160"/>
-        <c:axId val="137486336"/>
+        <c:axId val="151947136"/>
+        <c:axId val="151948672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137468160"/>
+        <c:axId val="151947136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -218,7 +254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137486336"/>
+        <c:crossAx val="151948672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -226,7 +262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137486336"/>
+        <c:axId val="151948672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -237,7 +273,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137468160"/>
+        <c:crossAx val="151947136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -273,6 +309,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Set work priority</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -286,7 +341,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$95,Sheet1!$B$96)</c:f>
+              <c:f>(Sheet1!$B$105,Sheet1!$B$106)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -300,7 +355,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$95,Sheet1!$F$96)</c:f>
+              <c:f>(Sheet1!$F$105,Sheet1!$F$106)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -324,11 +379,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="62884096"/>
-        <c:axId val="62886272"/>
+        <c:axId val="153063808"/>
+        <c:axId val="153065344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62884096"/>
+        <c:axId val="153063808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,7 +392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62886272"/>
+        <c:crossAx val="153065344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -345,7 +400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62886272"/>
+        <c:axId val="153065344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62884096"/>
+        <c:crossAx val="153063808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -392,6 +447,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Create work</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -405,7 +479,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$16,Sheet1!$B$17)</c:f>
+              <c:f>(Sheet1!$B$18,Sheet1!$B$19)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -419,7 +493,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$16,Sheet1!$F$17)</c:f>
+              <c:f>(Sheet1!$F$18,Sheet1!$F$19)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -443,11 +517,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="137960832"/>
-        <c:axId val="137962624"/>
+        <c:axId val="152378368"/>
+        <c:axId val="152380160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137960832"/>
+        <c:axId val="152378368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137962624"/>
+        <c:crossAx val="152380160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -464,7 +538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137962624"/>
+        <c:axId val="152380160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137960832"/>
+        <c:crossAx val="152378368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -511,6 +585,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Delete work</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -524,7 +617,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$16,Sheet1!$B$17)</c:f>
+              <c:f>(Sheet1!$B$18,Sheet1!$B$19)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -538,7 +631,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$16,Sheet1!$F$17)</c:f>
+              <c:f>(Sheet1!$F$18,Sheet1!$F$19)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -562,11 +655,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="61464576"/>
-        <c:axId val="61466112"/>
+        <c:axId val="152408448"/>
+        <c:axId val="152409984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61464576"/>
+        <c:axId val="152408448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61466112"/>
+        <c:crossAx val="152409984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -583,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61466112"/>
+        <c:axId val="152409984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61464576"/>
+        <c:crossAx val="152408448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -630,6 +723,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Create project</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -643,7 +755,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$35,Sheet1!$B$36)</c:f>
+              <c:f>(Sheet1!$B$39,Sheet1!$B$40)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -657,7 +769,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$35,Sheet1!$F$36)</c:f>
+              <c:f>(Sheet1!$F$39,Sheet1!$F$40)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -681,11 +793,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="62237696"/>
-        <c:axId val="62916864"/>
+        <c:axId val="152430080"/>
+        <c:axId val="152431616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62237696"/>
+        <c:axId val="152430080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,7 +806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62916864"/>
+        <c:crossAx val="152431616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -702,7 +814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62916864"/>
+        <c:axId val="152431616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,7 +825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62237696"/>
+        <c:crossAx val="152430080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -749,6 +861,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Delete project</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -762,7 +893,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$44,Sheet1!$B$45)</c:f>
+              <c:f>(Sheet1!$B$48,Sheet1!$B$49)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -776,7 +907,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$44,Sheet1!$F$45)</c:f>
+              <c:f>(Sheet1!$F$48,Sheet1!$F$49)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -800,11 +931,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="61455744"/>
-        <c:axId val="62223104"/>
+        <c:axId val="152447616"/>
+        <c:axId val="152465792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61455744"/>
+        <c:axId val="152447616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +944,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62223104"/>
+        <c:crossAx val="152465792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62223104"/>
+        <c:axId val="152465792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61455744"/>
+        <c:crossAx val="152447616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -868,6 +999,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Load dashboard</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -881,7 +1031,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$55,Sheet1!$B$56)</c:f>
+              <c:f>(Sheet1!$B$61,Sheet1!$B$62)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -895,7 +1045,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$55,Sheet1!$F$56)</c:f>
+              <c:f>(Sheet1!$F$61,Sheet1!$F$62)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -919,11 +1069,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="138193920"/>
-        <c:axId val="138381568"/>
+        <c:axId val="152568192"/>
+        <c:axId val="152569728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138193920"/>
+        <c:axId val="152568192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,7 +1082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138381568"/>
+        <c:crossAx val="152569728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -940,7 +1090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138381568"/>
+        <c:axId val="152569728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +1101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138193920"/>
+        <c:crossAx val="152568192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,6 +1137,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Change Password</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1000,7 +1169,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$65,Sheet1!$B$66)</c:f>
+              <c:f>(Sheet1!$B$73,Sheet1!$B$74)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1014,7 +1183,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$65,Sheet1!$F$66)</c:f>
+              <c:f>(Sheet1!$F$73,Sheet1!$F$74)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1038,11 +1207,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="138600448"/>
-        <c:axId val="138601984"/>
+        <c:axId val="152581632"/>
+        <c:axId val="152583168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138600448"/>
+        <c:axId val="152581632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1220,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138601984"/>
+        <c:crossAx val="152583168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1059,7 +1228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138601984"/>
+        <c:axId val="152583168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138600448"/>
+        <c:crossAx val="152581632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1106,6 +1275,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Login request</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1119,7 +1307,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$75,Sheet1!$B$76)</c:f>
+              <c:f>(Sheet1!$B$85,Sheet1!$B$86)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1133,7 +1321,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$75,Sheet1!$F$76)</c:f>
+              <c:f>(Sheet1!$F$85,Sheet1!$F$86)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1157,11 +1345,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="62712448"/>
-        <c:axId val="62748160"/>
+        <c:axId val="152603264"/>
+        <c:axId val="152613248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62712448"/>
+        <c:axId val="152603264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62748160"/>
+        <c:crossAx val="152613248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1178,7 +1366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62748160"/>
+        <c:axId val="152613248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,7 +1377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62712448"/>
+        <c:crossAx val="152603264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1225,6 +1413,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Logout request</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1238,7 +1445,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>(Sheet1!$B$85,Sheet1!$B$86)</c:f>
+              <c:f>(Sheet1!$B$95,Sheet1!$B$96)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1252,7 +1459,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$F$85,Sheet1!$F$86)</c:f>
+              <c:f>(Sheet1!$F$95,Sheet1!$F$96)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1276,11 +1483,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="61557760"/>
-        <c:axId val="62271872"/>
+        <c:axId val="152624128"/>
+        <c:axId val="153039616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61557760"/>
+        <c:axId val="152624128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,7 +1496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62271872"/>
+        <c:crossAx val="153039616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1297,7 +1504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62271872"/>
+        <c:axId val="153039616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61557760"/>
+        <c:crossAx val="152624128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1335,15 +1542,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1365,15 +1572,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1396,13 +1603,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1426,16 +1633,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1456,16 +1663,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1488,13 +1695,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1516,16 +1723,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1548,13 +1755,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1578,13 +1785,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1608,14 +1815,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1924,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F96"/>
+  <dimension ref="B3:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I99" sqref="I99"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,1014 +2143,1020 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>1.8356481481481479E-4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>3.8976851851851851E-4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>4.166435185185185E-4</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <f>AVERAGE(C5:E5)</f>
         <v>3.2999228395061723E-4</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>58</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>58</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>58</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <f>AVERAGE(C6:E6)</f>
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="7">
         <v>24246</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="7">
         <v>25823</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="7">
         <v>25823</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="7">
         <f>AVERAGE(C7:E7)</f>
         <v>25297.333333333332</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
         <v>1033083</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="7">
         <v>1032839</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="7">
         <v>1032846</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="7">
         <f>AVERAGE(C8:E8)</f>
         <v>1032922.6666666666</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1.3877314814814816E-5</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.1018518518518517E-5</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1.3877314814814816E-5</v>
+      </c>
+      <c r="F16" s="6">
+        <f>AVERAGE(C16:E16)</f>
+        <v>1.2924382716049384E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <f>AVERAGE(C17:E17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2506</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2506</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2506</v>
+      </c>
+      <c r="F18" s="7">
+        <f>AVERAGE(C18:E18)</f>
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2225</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2210</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2225</v>
+      </c>
+      <c r="F19" s="7">
+        <f>AVERAGE(C19:E19)</f>
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1.0787037037037037E-5</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1.082175925925926E-5</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1.0891203703703705E-5</v>
+      </c>
+      <c r="F27" s="6">
+        <f>AVERAGE(C27:E27)</f>
+        <v>1.0833333333333335E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5">
+        <v>3</v>
+      </c>
+      <c r="F28" s="5">
+        <f>AVERAGE(C28:E28)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2471</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2471</v>
+      </c>
+      <c r="E29" s="5">
+        <v>2471</v>
+      </c>
+      <c r="F29" s="7">
+        <f>AVERAGE(C29:E29)</f>
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2219</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2224</v>
+      </c>
+      <c r="E30" s="5">
+        <v>2224</v>
+      </c>
+      <c r="F30" s="7">
+        <f>AVERAGE(C30:E30)</f>
+        <v>2222.3333333333335</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F36" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1">
-        <v>1.3877314814814816E-5</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1.1018518518518517E-5</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1.3877314814814816E-5</v>
-      </c>
-      <c r="F14" s="1">
-        <f>AVERAGE(C14:E14)</f>
-        <v>1.2924382716049384E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C37" s="6">
+        <v>1.1238425925925927E-5</v>
+      </c>
+      <c r="D37" s="6">
+        <v>8.8888888888888883E-6</v>
+      </c>
+      <c r="E37" s="6">
+        <v>8.5185185185185192E-6</v>
+      </c>
+      <c r="F37" s="6">
+        <f>AVERAGE(C37:E37)</f>
+        <v>9.5486111111111109E-6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <f>AVERAGE(C15:E15)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>2</v>
+      </c>
+      <c r="F38" s="5">
+        <f>AVERAGE(C38:E38)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
-        <v>2506</v>
-      </c>
-      <c r="D16">
-        <v>2506</v>
-      </c>
-      <c r="E16">
-        <v>2506</v>
-      </c>
-      <c r="F16" s="2">
-        <f>AVERAGE(C16:E16)</f>
-        <v>2506</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>2225</v>
-      </c>
-      <c r="D17">
-        <v>2210</v>
-      </c>
-      <c r="E17">
-        <v>2225</v>
-      </c>
-      <c r="F17" s="2">
-        <f>AVERAGE(C17:E17)</f>
-        <v>2220</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1.0787037037037037E-5</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1.082175925925926E-5</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1.0891203703703705E-5</v>
-      </c>
-      <c r="F24" s="1">
-        <f>AVERAGE(C24:E24)</f>
-        <v>1.0833333333333335E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <f>AVERAGE(C25:E25)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26">
-        <v>2471</v>
-      </c>
-      <c r="D26">
-        <v>2471</v>
-      </c>
-      <c r="E26">
-        <v>2471</v>
-      </c>
-      <c r="F26" s="2">
-        <f>AVERAGE(C26:E26)</f>
-        <v>2471</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27">
-        <v>2219</v>
-      </c>
-      <c r="D27">
-        <v>2224</v>
-      </c>
-      <c r="E27">
-        <v>2224</v>
-      </c>
-      <c r="F27" s="2">
-        <f>AVERAGE(C27:E27)</f>
-        <v>2222.3333333333335</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1.1238425925925927E-5</v>
-      </c>
-      <c r="D33" s="1">
-        <v>8.8888888888888883E-6</v>
-      </c>
-      <c r="E33" s="1">
-        <v>8.5185185185185192E-6</v>
-      </c>
-      <c r="F33" s="1">
-        <f>AVERAGE(C33:E33)</f>
-        <v>9.5486111111111109E-6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34">
-        <f>AVERAGE(C34:E34)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35">
+      <c r="C39" s="5">
         <v>1708</v>
       </c>
-      <c r="D35">
+      <c r="D39" s="5">
         <v>1708</v>
       </c>
-      <c r="E35">
+      <c r="E39" s="5">
         <v>1708</v>
       </c>
-      <c r="F35" s="2">
-        <f>AVERAGE(C35:E35)</f>
+      <c r="F39" s="7">
+        <f>AVERAGE(C39:E39)</f>
         <v>1708</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36">
-        <v>1346</v>
-      </c>
-      <c r="D36">
-        <v>1351</v>
-      </c>
-      <c r="E36">
-        <v>1351</v>
-      </c>
-      <c r="F36" s="2">
-        <f>AVERAGE(C36:E36)</f>
-        <v>1349.3333333333333</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1346</v>
+      </c>
+      <c r="D40" s="5">
+        <v>1351</v>
+      </c>
+      <c r="E40" s="5">
+        <v>1351</v>
+      </c>
+      <c r="F40" s="7">
+        <f>AVERAGE(C40:E40)</f>
+        <v>1349.3333333333333</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E45" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F45" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C46" s="6">
         <v>2.2523148148148152E-5</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D46" s="6">
         <v>2.0902777777777778E-5</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E46" s="6">
         <v>1.9050925925925924E-5</v>
       </c>
-      <c r="F42" s="1">
-        <f>AVERAGE(C42:E42)</f>
+      <c r="F46" s="6">
+        <f>AVERAGE(C46:E46)</f>
         <v>2.0825617283950617E-5</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C43">
+      <c r="C47" s="5">
         <v>4</v>
       </c>
-      <c r="D43">
+      <c r="D47" s="5">
         <v>4</v>
       </c>
-      <c r="E43">
+      <c r="E47" s="5">
         <v>4</v>
       </c>
-      <c r="F43">
-        <f>AVERAGE(C43:E43)</f>
+      <c r="F47" s="5">
+        <f>AVERAGE(C47:E47)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C44">
+      <c r="C48" s="5">
         <v>3268</v>
       </c>
-      <c r="D44">
+      <c r="D48" s="5">
         <v>3268</v>
       </c>
-      <c r="E44">
+      <c r="E48" s="5">
         <v>3268</v>
       </c>
-      <c r="F44" s="2">
-        <f>AVERAGE(C44:E44)</f>
+      <c r="F48" s="7">
+        <f>AVERAGE(C48:E48)</f>
         <v>3268</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C45">
+      <c r="C49" s="5">
         <v>11127</v>
       </c>
-      <c r="D45">
+      <c r="D49" s="5">
         <v>10723</v>
       </c>
-      <c r="E45">
+      <c r="E49" s="5">
         <v>10319</v>
       </c>
-      <c r="F45" s="2">
-        <f>AVERAGE(C45:E45)</f>
+      <c r="F49" s="7">
+        <f>AVERAGE(C49:E49)</f>
         <v>10723</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="2"/>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="1"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C58" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D58" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E58" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F58" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C59" s="6">
         <v>4.9337962962962964E-4</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D59" s="6">
         <v>4.5409722222222227E-4</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E59" s="6">
         <v>4.9903935185185175E-4</v>
       </c>
-      <c r="F53" s="1">
-        <f>AVERAGE(C53:E53)</f>
+      <c r="F59" s="6">
+        <f>AVERAGE(C59:E59)</f>
         <v>4.8217206790123461E-4</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C54">
+      <c r="C60" s="5">
         <v>66</v>
       </c>
-      <c r="D54">
-        <v>67</v>
-      </c>
-      <c r="E54">
+      <c r="D60" s="5">
         <v>66</v>
       </c>
-      <c r="F54">
-        <f>AVERAGE(C54:E54)</f>
-        <v>66.333333333333329</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55">
-        <v>53408</v>
-      </c>
-      <c r="D55">
-        <v>54224</v>
-      </c>
-      <c r="E55">
-        <v>53408</v>
-      </c>
-      <c r="F55" s="2">
-        <f>AVERAGE(C55:E55)</f>
-        <v>53680</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56">
-        <v>1054212</v>
-      </c>
-      <c r="D56">
-        <v>1055197</v>
-      </c>
-      <c r="E56">
-        <v>1054534</v>
-      </c>
-      <c r="F56" s="2">
-        <f>AVERAGE(C56:E56)</f>
-        <v>1054647.6666666667</v>
+      <c r="E60" s="5">
+        <v>66</v>
+      </c>
+      <c r="F60" s="5">
+        <f>AVERAGE(C60:E60)</f>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="C61" s="5">
+        <v>53408</v>
+      </c>
+      <c r="D61" s="5">
+        <v>54224</v>
+      </c>
+      <c r="E61" s="5">
+        <v>53408</v>
+      </c>
+      <c r="F61" s="7">
+        <f>AVERAGE(C61:E61)</f>
+        <v>53680</v>
+      </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1054212</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1055197</v>
+      </c>
+      <c r="E62" s="5">
+        <v>1054534</v>
+      </c>
+      <c r="F62" s="7">
+        <f>AVERAGE(C62:E62)</f>
+        <v>1054647.6666666667</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C70" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D70" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E70" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F70" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="1">
-        <v>5.9282407407407397E-5</v>
-      </c>
-      <c r="D63" s="1">
-        <v>3.1203703703703706E-5</v>
-      </c>
-      <c r="E63" s="1">
-        <v>3.6527777777777775E-5</v>
-      </c>
-      <c r="F63" s="1">
-        <f>AVERAGE(C63:E63)</f>
-        <v>4.2337962962962962E-5</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64">
-        <v>5</v>
-      </c>
-      <c r="D64">
-        <v>5</v>
-      </c>
-      <c r="E64">
-        <v>5</v>
-      </c>
-      <c r="F64">
-        <f>AVERAGE(C64:E64)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65">
-        <v>4683</v>
-      </c>
-      <c r="D65">
-        <v>4683</v>
-      </c>
-      <c r="E65">
-        <v>4683</v>
-      </c>
-      <c r="F65" s="2">
-        <f>AVERAGE(C65:E65)</f>
-        <v>4683</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66">
-        <v>10341</v>
-      </c>
-      <c r="D66">
-        <v>10366</v>
-      </c>
-      <c r="E66">
-        <v>10346</v>
-      </c>
-      <c r="F66" s="2">
-        <f>AVERAGE(C66:E66)</f>
-        <v>10351</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="C71" s="6">
+        <v>5.9282407407407397E-5</v>
+      </c>
+      <c r="D71" s="6">
+        <v>3.1203703703703706E-5</v>
+      </c>
+      <c r="E71" s="6">
+        <v>3.6527777777777775E-5</v>
+      </c>
+      <c r="F71" s="6">
+        <f>AVERAGE(C71:E71)</f>
+        <v>4.2337962962962962E-5</v>
+      </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="5">
+        <v>5</v>
+      </c>
+      <c r="D72" s="5">
+        <v>5</v>
+      </c>
+      <c r="E72" s="5">
+        <v>5</v>
+      </c>
+      <c r="F72" s="5">
+        <f>AVERAGE(C72:E72)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="5">
+        <v>4683</v>
+      </c>
+      <c r="D73" s="5">
+        <v>4683</v>
+      </c>
+      <c r="E73" s="5">
+        <v>4683</v>
+      </c>
+      <c r="F73" s="7">
+        <f>AVERAGE(C73:E73)</f>
+        <v>4683</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" s="5">
+        <v>10341</v>
+      </c>
+      <c r="D74" s="5">
+        <v>10366</v>
+      </c>
+      <c r="E74" s="5">
+        <v>10346</v>
+      </c>
+      <c r="F74" s="7">
+        <f>AVERAGE(C74:E74)</f>
+        <v>10351</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C82" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D82" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E82" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F82" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C83" s="6">
         <v>2.4537037037037038E-5</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D83" s="6">
         <v>3.2673611111111114E-5</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E83" s="6">
         <v>3.0046296296296299E-5</v>
       </c>
-      <c r="F73" s="1">
-        <f>AVERAGE(C73:E73)</f>
+      <c r="F83" s="6">
+        <f>AVERAGE(C83:E83)</f>
         <v>2.9085648148148149E-5</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C74">
+      <c r="C84" s="5">
         <v>2</v>
       </c>
-      <c r="D74">
+      <c r="D84" s="5">
         <v>2</v>
       </c>
-      <c r="E74">
+      <c r="E84" s="5">
         <v>2</v>
       </c>
-      <c r="F74">
-        <f>AVERAGE(C74:E74)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75">
-        <v>5195</v>
-      </c>
-      <c r="D75">
-        <v>5195</v>
-      </c>
-      <c r="E75">
-        <v>5195</v>
-      </c>
-      <c r="F75" s="2">
-        <f>AVERAGE(C75:E75)</f>
-        <v>5195</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76">
-        <v>91631</v>
-      </c>
-      <c r="D76">
-        <v>91631</v>
-      </c>
-      <c r="E76">
-        <v>91631</v>
-      </c>
-      <c r="F76" s="2">
-        <f>AVERAGE(C76:E76)</f>
-        <v>91631</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>4</v>
-      </c>
-      <c r="C83" s="1">
-        <v>2.4537037037037038E-5</v>
-      </c>
-      <c r="D83" s="1">
-        <v>2.8622685185185185E-5</v>
-      </c>
-      <c r="E83" s="1">
-        <v>1.9652777777777775E-5</v>
-      </c>
-      <c r="F83" s="1">
-        <f>AVERAGE(C83:E83)</f>
-        <v>2.4270833333333335E-5</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84">
-        <v>2</v>
-      </c>
-      <c r="D84">
-        <v>2</v>
-      </c>
-      <c r="E84">
-        <v>2</v>
-      </c>
-      <c r="F84">
+      <c r="F84" s="5">
         <f>AVERAGE(C84:E84)</f>
         <v>2</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="5">
         <v>5195</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="5">
+        <v>5195</v>
+      </c>
+      <c r="E85" s="5">
+        <v>5195</v>
+      </c>
+      <c r="F85" s="7">
+        <f>AVERAGE(C85:E85)</f>
+        <v>5195</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="5">
+        <v>91631</v>
+      </c>
+      <c r="D86" s="5">
+        <v>91631</v>
+      </c>
+      <c r="E86" s="5">
+        <v>91631</v>
+      </c>
+      <c r="F86" s="7">
+        <f>AVERAGE(C86:E86)</f>
+        <v>91631</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="6">
+        <v>2.4537037037037038E-5</v>
+      </c>
+      <c r="D93" s="6">
+        <v>2.8622685185185185E-5</v>
+      </c>
+      <c r="E93" s="6">
+        <v>1.9652777777777775E-5</v>
+      </c>
+      <c r="F93" s="6">
+        <f>AVERAGE(C93:E93)</f>
+        <v>2.4270833333333335E-5</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="5">
+        <v>2</v>
+      </c>
+      <c r="D94" s="5">
+        <v>2</v>
+      </c>
+      <c r="E94" s="5">
+        <v>2</v>
+      </c>
+      <c r="F94" s="5">
+        <f>AVERAGE(C94:E94)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="5">
+        <v>5195</v>
+      </c>
+      <c r="D95" s="5">
         <v>15269</v>
       </c>
-      <c r="E85">
+      <c r="E95" s="5">
         <v>15269</v>
       </c>
-      <c r="F85" s="2">
-        <f>AVERAGE(C85:E85)</f>
+      <c r="F95" s="7">
+        <f>AVERAGE(C95:E95)</f>
         <v>11911</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C86">
+      <c r="C96" s="5">
         <v>91631</v>
       </c>
-      <c r="D86">
+      <c r="D96" s="5">
         <v>39517</v>
       </c>
-      <c r="E86">
+      <c r="E96" s="5">
         <v>39517</v>
       </c>
-      <c r="F86" s="2">
-        <f>AVERAGE(C86:E86)</f>
+      <c r="F96" s="7">
+        <f>AVERAGE(C96:E96)</f>
         <v>56888.333333333336</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C102" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D102" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E102" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F92" s="3" t="s">
+      <c r="F102" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C103" s="6">
         <v>5.5671296296296303E-6</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D103" s="6">
         <v>5.4629629629629623E-6</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E103" s="6">
         <v>6.6435185185185176E-6</v>
       </c>
-      <c r="F93" s="1">
-        <f>AVERAGE(C93:E93)</f>
+      <c r="F103" s="6">
+        <f>AVERAGE(C103:E103)</f>
         <v>5.8912037037037031E-6</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C94">
+      <c r="C104" s="5">
         <v>1</v>
       </c>
-      <c r="D94">
+      <c r="D104" s="5">
         <v>1</v>
       </c>
-      <c r="E94">
+      <c r="E104" s="5">
         <v>1</v>
       </c>
-      <c r="F94">
-        <f>AVERAGE(C94:E94)</f>
+      <c r="F104" s="5">
+        <f>AVERAGE(C104:E104)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C95">
+      <c r="C105" s="5">
         <v>899</v>
       </c>
-      <c r="D95">
+      <c r="D105" s="5">
         <v>899</v>
       </c>
-      <c r="E95">
+      <c r="E105" s="5">
         <v>899</v>
       </c>
-      <c r="F95" s="2">
-        <f>AVERAGE(C95:E95)</f>
+      <c r="F105" s="7">
+        <f>AVERAGE(C105:E105)</f>
         <v>899</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C96">
+      <c r="C106" s="5">
         <v>1041</v>
       </c>
-      <c r="D96">
+      <c r="D106" s="5">
         <v>1049</v>
       </c>
-      <c r="E96">
+      <c r="E106" s="5">
         <v>1049</v>
       </c>
-      <c r="F96" s="2">
-        <f>AVERAGE(C96:E96)</f>
+      <c r="F106" s="7">
+        <f>AVERAGE(C106:E106)</f>
         <v>1046.3333333333333</v>
       </c>
     </row>

</xml_diff>